<commit_message>
Get Data with dataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/DataCate.xlsx
+++ b/src/test/resources/datatest/DataCate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Git\ProjectTestCMS\src\test\resources\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1292FDCD-A157-44A5-89EA-9C5394458CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1A9B9F-C223-41AB-8056-B2BF4381B933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="3915" windowWidth="16500" windowHeight="8655" xr2:uid="{E621E065-9829-4F78-8EA1-FF220EE35D9A}"/>
+    <workbookView xWindow="4200" yWindow="1425" windowWidth="18030" windowHeight="13620" xr2:uid="{E621E065-9829-4F78-8EA1-FF220EE35D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>NAME</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Capacity</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67640CA-51D4-4C4B-B5FA-E366C23314C4}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD9"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +500,31 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>